<commit_message>
budget, AT connectors, 18 pin on CEN>HIP loom
</commit_message>
<xml_diff>
--- a/MCHA Budget.xlsx
+++ b/MCHA Budget.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Github\NU-Racing-Lead-MCHA-2025\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Uni\NU Teams\2025 Lead MCHA\NU-Racing-Lead-MCHA-2025\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{212EB9D2-D08F-45DB-BBB2-7AA6D1787E34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5FCB2DA-DB89-40B6-BB0C-E6EE936DE421}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{C94B0C8E-4BB7-41BB-BABD-F0454CF43B33}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{C94B0C8E-4BB7-41BB-BABD-F0454CF43B33}"/>
   </bookViews>
   <sheets>
     <sheet name="Splurge Budget" sheetId="3" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="96">
   <si>
     <t>MCHA</t>
   </si>
@@ -317,6 +317,15 @@
   </si>
   <si>
     <t>Without MC or Motor</t>
+  </si>
+  <si>
+    <t>*taken from my boots order from 2024, 5x204W511-25-0, 4x202K111-25-0, 10x202K232-25-0, 7x202A132-25-0</t>
+  </si>
+  <si>
+    <t>*taken from my boots order from 2024, plus some room for extras, 5x204W511-25-0, 4x202K111-25-0, 10x202K232-25-0, 7x202A132-25-0</t>
+  </si>
+  <si>
+    <t>*2 teensys/board, 4 boards</t>
   </si>
 </sst>
 </file>
@@ -593,12 +602,6 @@
   </cellStyleXfs>
   <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -629,9 +632,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="4"/>
     <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -648,6 +648,15 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="3" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="3" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="40% - Accent4" xfId="3" builtinId="43"/>
@@ -668,67 +677,20 @@
       </border>
     </dxf>
     <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
           <color indexed="64"/>
         </left>
         <right/>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right/>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="34" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
         <top style="thin">
           <color indexed="64"/>
         </top>
@@ -742,14 +704,6 @@
           <bgColor auto="1"/>
         </patternFill>
       </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
@@ -762,6 +716,18 @@
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
       </border>
     </dxf>
     <dxf>
@@ -784,6 +750,21 @@
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="34" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
       </border>
     </dxf>
     <dxf>
@@ -822,6 +803,34 @@
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
       </border>
     </dxf>
     <dxf>
@@ -869,13 +878,6 @@
     </dxf>
     <dxf>
       <border outline="0">
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
         <left style="thin">
           <color indexed="64"/>
         </left>
@@ -897,6 +899,13 @@
           <bgColor auto="1"/>
         </patternFill>
       </fill>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
     </dxf>
     <dxf>
       <font>
@@ -936,14 +945,14 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{632ABA69-513E-472D-BD72-34E9E5AD39D8}" name="Table1" displayName="Table1" ref="B37:F45" totalsRowCount="1" headerRowDxfId="14" dataDxfId="13" headerRowBorderDxfId="11" tableBorderDxfId="12" totalsRowBorderDxfId="10">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{632ABA69-513E-472D-BD72-34E9E5AD39D8}" name="Table1" displayName="Table1" ref="B37:F45" totalsRowCount="1" headerRowDxfId="14" dataDxfId="12" headerRowBorderDxfId="13" tableBorderDxfId="11" totalsRowBorderDxfId="10">
   <autoFilter ref="B37:F44" xr:uid="{632ABA69-513E-472D-BD72-34E9E5AD39D8}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{856A96CB-9007-432B-9D91-DDFF63C2D973}" name="Column1" totalsRowLabel="Total" dataDxfId="9" totalsRowDxfId="4"/>
-    <tableColumn id="2" xr3:uid="{D57FFE14-206F-419E-8F97-4FC39112C115}" name="Cost" totalsRowFunction="sum" dataDxfId="8" totalsRowDxfId="3" dataCellStyle="Currency"/>
-    <tableColumn id="3" xr3:uid="{6634B4BD-1EB1-4132-ACE8-4FA0828FB972}" name="Notes" dataDxfId="7" totalsRowDxfId="2"/>
-    <tableColumn id="6" xr3:uid="{FD5BACA0-F193-467D-AE15-943238B71206}" name="Month to be purchased" dataDxfId="6" totalsRowDxfId="1"/>
-    <tableColumn id="4" xr3:uid="{B9733096-4A0E-4C53-8006-32BE6A5CBEF2}" name="Column2" dataDxfId="5" totalsRowDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{856A96CB-9007-432B-9D91-DDFF63C2D973}" name="Column1" totalsRowLabel="Total" dataDxfId="9" totalsRowDxfId="8"/>
+    <tableColumn id="2" xr3:uid="{D57FFE14-206F-419E-8F97-4FC39112C115}" name="Cost" totalsRowFunction="sum" dataDxfId="7" totalsRowDxfId="6" dataCellStyle="Currency"/>
+    <tableColumn id="3" xr3:uid="{6634B4BD-1EB1-4132-ACE8-4FA0828FB972}" name="Notes" dataDxfId="5" totalsRowDxfId="4"/>
+    <tableColumn id="6" xr3:uid="{FD5BACA0-F193-467D-AE15-943238B71206}" name="Month to be purchased" dataDxfId="3" totalsRowDxfId="2"/>
+    <tableColumn id="4" xr3:uid="{B9733096-4A0E-4C53-8006-32BE6A5CBEF2}" name="Column2" dataDxfId="1" totalsRowDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1268,26 +1277,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C48F2814-B5D2-412D-912B-E55D56A02CFA}">
   <dimension ref="A1:G33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K12" sqref="K12"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="26.5703125" customWidth="1"/>
-    <col min="2" max="2" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="23.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="73.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="26.5546875" customWidth="1"/>
+    <col min="2" max="2" width="14.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="73.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="23" t="s">
+    <row r="1" spans="1:7" ht="37.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="20" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C2" t="s">
         <v>72</v>
       </c>
@@ -1304,29 +1313,29 @@
         <v>73</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>53</v>
       </c>
-      <c r="B3" s="26" t="s">
+      <c r="B3" s="23" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="30"/>
-      <c r="D3" s="30"/>
-      <c r="E3" s="30"/>
-      <c r="F3" s="30"/>
-      <c r="G3" s="30"/>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C3" s="27"/>
+      <c r="D3" s="27"/>
+      <c r="E3" s="27"/>
+      <c r="F3" s="27"/>
+      <c r="G3" s="27"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4">
         <f>21+2+2+2+2+1+1+2+2+2+1+1+1+1+1+1+1+6+1+1+1+1+1+5+3</f>
         <v>63</v>
       </c>
-      <c r="B4" s="32"/>
-      <c r="C4" s="27" t="s">
+      <c r="B4" s="29"/>
+      <c r="C4" s="24" t="s">
         <v>83</v>
       </c>
-      <c r="D4" s="25">
+      <c r="D4" s="22">
         <f>60</f>
         <v>60</v>
       </c>
@@ -1334,12 +1343,12 @@
         <v>84</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B5" s="32"/>
-      <c r="C5" s="27" t="s">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B5" s="29"/>
+      <c r="C5" s="24" t="s">
         <v>31</v>
       </c>
-      <c r="D5" s="25">
+      <c r="D5" s="22">
         <f>60+30</f>
         <v>90</v>
       </c>
@@ -1347,16 +1356,16 @@
         <v>65</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B6" s="32"/>
-      <c r="C6" s="27" t="s">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B6" s="29"/>
+      <c r="C6" s="24" t="s">
         <v>32</v>
       </c>
-      <c r="D6" s="25">
+      <c r="D6" s="22">
         <f>2*120</f>
         <v>240</v>
       </c>
-      <c r="E6" s="25">
+      <c r="E6" s="22">
         <f>D6+D6*0.5</f>
         <v>360</v>
       </c>
@@ -1364,38 +1373,38 @@
         <v>66</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B7" s="32"/>
-      <c r="C7" s="27" t="s">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B7" s="29"/>
+      <c r="C7" s="24" t="s">
         <v>30</v>
       </c>
-      <c r="D7" s="24">
+      <c r="D7" s="21">
         <f>80+35+60+90*2</f>
         <v>355</v>
       </c>
-      <c r="F7" s="20" t="s">
+      <c r="F7" s="18" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B8" s="32"/>
-      <c r="C8" s="27" t="s">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B8" s="29"/>
+      <c r="C8" s="24" t="s">
         <v>60</v>
       </c>
-      <c r="D8" s="24">
+      <c r="D8" s="21">
         <f>55+65+22+97+2*30</f>
         <v>299</v>
       </c>
-      <c r="F8" s="20" t="s">
+      <c r="F8" s="18" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B9" s="32"/>
-      <c r="C9" s="27" t="s">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B9" s="29"/>
+      <c r="C9" s="24" t="s">
         <v>33</v>
       </c>
-      <c r="D9" s="25">
+      <c r="D9" s="22">
         <f>3*80+30</f>
         <v>270</v>
       </c>
@@ -1403,46 +1412,46 @@
         <v>68</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B10" s="32"/>
-      <c r="C10" s="27" t="s">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B10" s="29"/>
+      <c r="C10" s="24" t="s">
         <v>34</v>
       </c>
-      <c r="D10" s="25">
+      <c r="D10" s="22">
         <v>800</v>
       </c>
       <c r="F10" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B11" s="32"/>
-      <c r="C11" s="27" t="s">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B11" s="29"/>
+      <c r="C11" s="24" t="s">
         <v>35</v>
       </c>
-      <c r="D11" s="25">
+      <c r="D11" s="22">
         <v>200</v>
       </c>
       <c r="F11" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B12" s="26" t="s">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B12" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="C12" s="28"/>
-      <c r="D12" s="29"/>
-      <c r="E12" s="30"/>
-      <c r="F12" s="30"/>
-      <c r="G12" s="30"/>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B13" s="32"/>
-      <c r="C13" s="27" t="s">
+      <c r="C12" s="25"/>
+      <c r="D12" s="26"/>
+      <c r="E12" s="27"/>
+      <c r="F12" s="27"/>
+      <c r="G12" s="27"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B13" s="29"/>
+      <c r="C13" s="24" t="s">
         <v>36</v>
       </c>
-      <c r="D13" s="25">
+      <c r="D13" s="22">
         <f>44.95*3*4</f>
         <v>539.40000000000009</v>
       </c>
@@ -1450,12 +1459,12 @@
         <v>44</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B14" s="32"/>
-      <c r="C14" s="27" t="s">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B14" s="29"/>
+      <c r="C14" s="24" t="s">
         <v>37</v>
       </c>
-      <c r="D14" s="25">
+      <c r="D14" s="22">
         <f>2.65*63</f>
         <v>166.95</v>
       </c>
@@ -1463,78 +1472,79 @@
         <v>43</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B15" s="32"/>
-      <c r="C15" s="27" t="s">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B15" s="29"/>
+      <c r="C15" s="24" t="s">
         <v>38</v>
       </c>
-      <c r="D15" s="25">
+      <c r="D15" s="22">
         <f>40*12</f>
         <v>480</v>
       </c>
       <c r="F15" t="s">
         <v>42</v>
       </c>
-      <c r="G15" s="22" t="s">
+      <c r="G15" s="19" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B16" s="32"/>
-      <c r="C16" s="27" t="s">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B16" s="29"/>
+      <c r="C16" s="24" t="s">
         <v>39</v>
       </c>
-      <c r="D16" s="25">
+      <c r="D16" s="22">
+        <f>5*21+4*24+10*31+7*27+300</f>
         <v>1000</v>
       </c>
       <c r="F16" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B17" s="32"/>
-      <c r="C17" s="27" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="17" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B17" s="29"/>
+      <c r="C17" s="24" t="s">
         <v>40</v>
       </c>
-      <c r="D17" s="25">
+      <c r="D17" s="22">
         <v>200</v>
       </c>
       <c r="F17" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B18" s="31" t="s">
+    <row r="18" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B18" s="28" t="s">
         <v>70</v>
       </c>
-      <c r="C18" s="28"/>
-      <c r="D18" s="29"/>
-      <c r="E18" s="30"/>
-      <c r="F18" s="30"/>
-      <c r="G18" s="30"/>
-    </row>
-    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B19" s="32"/>
-      <c r="C19" s="27" t="s">
+      <c r="C18" s="25"/>
+      <c r="D18" s="26"/>
+      <c r="E18" s="27"/>
+      <c r="F18" s="27"/>
+      <c r="G18" s="27"/>
+    </row>
+    <row r="19" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B19" s="29"/>
+      <c r="C19" s="24" t="s">
         <v>48</v>
       </c>
-      <c r="D19" s="25">
+      <c r="D19" s="22">
         <f>4*37+2*40+2*65</f>
         <v>358</v>
       </c>
       <c r="F19" t="s">
         <v>50</v>
       </c>
-      <c r="G19" s="22" t="s">
+      <c r="G19" s="19" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="20" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B20" s="32"/>
-      <c r="C20" s="27" t="s">
+    <row r="20" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B20" s="29"/>
+      <c r="C20" s="24" t="s">
         <v>49</v>
       </c>
-      <c r="D20" s="25">
+      <c r="D20" s="22">
         <f>2*40+2*65+1*70+1*122</f>
         <v>402</v>
       </c>
@@ -1542,155 +1552,155 @@
         <v>51</v>
       </c>
     </row>
-    <row r="21" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B21" s="32"/>
-      <c r="C21" s="27" t="s">
+    <row r="21" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B21" s="29"/>
+      <c r="C21" s="24" t="s">
         <v>52</v>
       </c>
-      <c r="D21" s="25">
+      <c r="D21" s="22">
         <v>13400</v>
       </c>
       <c r="F21" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="22" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B22" s="32"/>
-      <c r="C22" s="27" t="s">
+    <row r="22" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B22" s="29"/>
+      <c r="C22" s="24" t="s">
         <v>90</v>
       </c>
-      <c r="D22" s="25">
+      <c r="D22" s="22">
         <v>6500</v>
       </c>
       <c r="F22" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="23" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B23" s="33" t="s">
+    <row r="23" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B23" s="30" t="s">
         <v>74</v>
       </c>
-      <c r="C23" s="28"/>
-      <c r="D23" s="29"/>
-      <c r="E23" s="30"/>
-      <c r="F23" s="30"/>
-      <c r="G23" s="30"/>
-    </row>
-    <row r="24" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B24" s="32"/>
-      <c r="C24" s="27" t="s">
+      <c r="C23" s="25"/>
+      <c r="D23" s="26"/>
+      <c r="E23" s="27"/>
+      <c r="F23" s="27"/>
+      <c r="G23" s="27"/>
+    </row>
+    <row r="24" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B24" s="29"/>
+      <c r="C24" s="24" t="s">
         <v>75</v>
       </c>
-      <c r="D24" s="25">
+      <c r="D24" s="22">
         <v>100</v>
       </c>
       <c r="F24" t="s">
         <v>76</v>
       </c>
-      <c r="G24" s="22" t="s">
+      <c r="G24" s="19" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="25" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B25" s="26" t="s">
+    <row r="25" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B25" s="23" t="s">
         <v>18</v>
       </c>
-      <c r="C25" s="30"/>
-      <c r="D25" s="29"/>
-      <c r="E25" s="30"/>
-      <c r="F25" s="30"/>
-      <c r="G25" s="30"/>
-    </row>
-    <row r="26" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B26" s="32"/>
-      <c r="C26" s="27" t="s">
+      <c r="C25" s="27"/>
+      <c r="D25" s="26"/>
+      <c r="E25" s="27"/>
+      <c r="F25" s="27"/>
+      <c r="G25" s="27"/>
+    </row>
+    <row r="26" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B26" s="29"/>
+      <c r="C26" s="24" t="s">
         <v>82</v>
       </c>
-      <c r="D26" s="25">
+      <c r="D26" s="22">
         <f>4*66</f>
         <v>264</v>
       </c>
       <c r="F26" t="s">
         <v>55</v>
       </c>
-      <c r="G26" s="22" t="s">
+      <c r="G26" s="19" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="27" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B27" s="31" t="s">
+    <row r="27" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B27" s="28" t="s">
         <v>69</v>
       </c>
-      <c r="C27" s="30"/>
-      <c r="D27" s="29"/>
-      <c r="E27" s="30"/>
-      <c r="F27" s="30"/>
-      <c r="G27" s="30"/>
-    </row>
-    <row r="28" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B28" s="32"/>
-      <c r="C28" s="27" t="s">
+      <c r="C27" s="27"/>
+      <c r="D27" s="26"/>
+      <c r="E27" s="27"/>
+      <c r="F27" s="27"/>
+      <c r="G27" s="27"/>
+    </row>
+    <row r="28" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B28" s="29"/>
+      <c r="C28" s="24" t="s">
         <v>56</v>
       </c>
-      <c r="D28" s="25">
+      <c r="D28" s="22">
         <v>5000</v>
       </c>
       <c r="F28" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="29" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B29" s="32"/>
-      <c r="C29" s="27" t="s">
+    <row r="29" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B29" s="29"/>
+      <c r="C29" s="24" t="s">
         <v>78</v>
       </c>
-      <c r="D29" s="25">
+      <c r="D29" s="22">
         <f>42+50</f>
         <v>92</v>
       </c>
       <c r="F29" t="s">
         <v>80</v>
       </c>
-      <c r="G29" s="22" t="s">
+      <c r="G29" s="19" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="30" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B30" s="26" t="s">
+    <row r="30" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B30" s="23" t="s">
         <v>28</v>
       </c>
-      <c r="C30" s="30"/>
-      <c r="D30" s="29"/>
-      <c r="E30" s="30"/>
-      <c r="F30" s="30"/>
-      <c r="G30" s="30"/>
-    </row>
-    <row r="31" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B31" s="32"/>
-      <c r="C31" s="27" t="s">
+      <c r="C30" s="27"/>
+      <c r="D30" s="26"/>
+      <c r="E30" s="27"/>
+      <c r="F30" s="27"/>
+      <c r="G30" s="27"/>
+    </row>
+    <row r="31" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B31" s="29"/>
+      <c r="C31" s="24" t="s">
         <v>59</v>
       </c>
-      <c r="D31" s="25">
+      <c r="D31" s="22">
         <f>SUM(D4:D29)</f>
         <v>30816.35</v>
       </c>
     </row>
-    <row r="32" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B32" s="32"/>
-      <c r="C32" s="27" t="s">
+    <row r="32" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B32" s="29"/>
+      <c r="C32" s="24" t="s">
         <v>58</v>
       </c>
-      <c r="D32" s="25">
+      <c r="D32" s="22">
         <f>D31-D21</f>
         <v>17416.349999999999</v>
       </c>
     </row>
-    <row r="33" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B33" s="32"/>
-      <c r="C33" s="27" t="s">
+    <row r="33" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B33" s="29"/>
+      <c r="C33" s="24" t="s">
         <v>92</v>
       </c>
-      <c r="D33" s="25">
+      <c r="D33" s="22">
         <f>D31-D22-D21</f>
         <v>10916.349999999999</v>
       </c>
@@ -1711,33 +1721,33 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C2DAFC3-A69B-479A-8EED-66262DCE6CA9}">
   <dimension ref="A1:H45"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="26.7109375" customWidth="1"/>
-    <col min="2" max="2" width="17.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="23.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.7109375" customWidth="1"/>
-    <col min="5" max="5" width="10.42578125" customWidth="1"/>
-    <col min="6" max="6" width="68.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="23.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="68.7109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="24.28515625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="26.6640625" customWidth="1"/>
+    <col min="2" max="2" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.6640625" customWidth="1"/>
+    <col min="5" max="5" width="10.44140625" customWidth="1"/>
+    <col min="6" max="6" width="68.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="23.44140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="68.6640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="24.33203125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="23" t="s">
+    <row r="1" spans="1:7" ht="36.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="20" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C2" t="s">
         <v>72</v>
       </c>
@@ -1754,37 +1764,37 @@
         <v>73</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>53</v>
       </c>
-      <c r="B3" s="26" t="s">
+      <c r="B3" s="23" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="30"/>
-      <c r="D3" s="30"/>
-      <c r="E3" s="30"/>
-      <c r="F3" s="30"/>
-      <c r="G3" s="30"/>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B4" s="32"/>
-      <c r="C4" s="27" t="s">
+      <c r="C3" s="27"/>
+      <c r="D3" s="27"/>
+      <c r="E3" s="27"/>
+      <c r="F3" s="27"/>
+      <c r="G3" s="27"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B4" s="29"/>
+      <c r="C4" s="24" t="s">
         <v>83</v>
       </c>
-      <c r="D4" s="25">
+      <c r="D4" s="22">
         <v>60</v>
       </c>
       <c r="F4" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B5" s="32"/>
-      <c r="C5" s="27" t="s">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B5" s="29"/>
+      <c r="C5" s="24" t="s">
         <v>31</v>
       </c>
-      <c r="D5" s="25">
+      <c r="D5" s="22">
         <f>60+30</f>
         <v>90</v>
       </c>
@@ -1792,16 +1802,16 @@
         <v>65</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B6" s="32"/>
-      <c r="C6" s="27" t="s">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B6" s="29"/>
+      <c r="C6" s="24" t="s">
         <v>32</v>
       </c>
-      <c r="D6" s="25">
+      <c r="D6" s="22">
         <f>2*120</f>
         <v>240</v>
       </c>
-      <c r="E6" s="25">
+      <c r="E6" s="22">
         <f>D6+D6*0.5</f>
         <v>360</v>
       </c>
@@ -1809,42 +1819,42 @@
         <v>66</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7">
         <f>21+2+2+2+2+1+1+2+2+2+1+1+1+1+1+1+1+6+1+1+1+1+1+5+3</f>
         <v>63</v>
       </c>
-      <c r="B7" s="32"/>
-      <c r="C7" s="27" t="s">
+      <c r="B7" s="29"/>
+      <c r="C7" s="24" t="s">
         <v>30</v>
       </c>
-      <c r="D7" s="24">
+      <c r="D7" s="21">
         <f>80+35+60</f>
         <v>175</v>
       </c>
-      <c r="F7" s="20" t="s">
+      <c r="F7" s="18" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B8" s="32"/>
-      <c r="C8" s="27" t="s">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B8" s="29"/>
+      <c r="C8" s="24" t="s">
         <v>60</v>
       </c>
-      <c r="D8" s="24">
+      <c r="D8" s="21">
         <f>55+65+22+97+2*30</f>
         <v>299</v>
       </c>
-      <c r="F8" s="20" t="s">
+      <c r="F8" s="18" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B9" s="32"/>
-      <c r="C9" s="27" t="s">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B9" s="29"/>
+      <c r="C9" s="24" t="s">
         <v>33</v>
       </c>
-      <c r="D9" s="25">
+      <c r="D9" s="22">
         <f>3*80</f>
         <v>240</v>
       </c>
@@ -1852,46 +1862,46 @@
         <v>67</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B10" s="32"/>
-      <c r="C10" s="27" t="s">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B10" s="29"/>
+      <c r="C10" s="24" t="s">
         <v>34</v>
       </c>
-      <c r="D10" s="25">
+      <c r="D10" s="22">
         <v>800</v>
       </c>
       <c r="F10" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B11" s="32"/>
-      <c r="C11" s="27" t="s">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B11" s="29"/>
+      <c r="C11" s="24" t="s">
         <v>35</v>
       </c>
-      <c r="D11" s="25">
+      <c r="D11" s="22">
         <v>200</v>
       </c>
       <c r="F11" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B12" s="26" t="s">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B12" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="C12" s="28"/>
-      <c r="D12" s="29"/>
-      <c r="E12" s="30"/>
-      <c r="F12" s="30"/>
-      <c r="G12" s="30"/>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B13" s="32"/>
-      <c r="C13" s="27" t="s">
+      <c r="C12" s="25"/>
+      <c r="D12" s="26"/>
+      <c r="E12" s="27"/>
+      <c r="F12" s="27"/>
+      <c r="G12" s="27"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B13" s="29"/>
+      <c r="C13" s="24" t="s">
         <v>36</v>
       </c>
-      <c r="D13" s="25">
+      <c r="D13" s="22">
         <f>44.95*3*4</f>
         <v>539.40000000000009</v>
       </c>
@@ -1899,12 +1909,12 @@
         <v>44</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B14" s="32"/>
-      <c r="C14" s="27" t="s">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B14" s="29"/>
+      <c r="C14" s="24" t="s">
         <v>37</v>
       </c>
-      <c r="D14" s="25">
+      <c r="D14" s="22">
         <f>2.65*63</f>
         <v>166.95</v>
       </c>
@@ -1912,78 +1922,79 @@
         <v>43</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B15" s="32"/>
-      <c r="C15" s="27" t="s">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B15" s="29"/>
+      <c r="C15" s="24" t="s">
         <v>38</v>
       </c>
-      <c r="D15" s="25">
+      <c r="D15" s="22">
         <f>40*12</f>
         <v>480</v>
       </c>
       <c r="F15" t="s">
         <v>42</v>
       </c>
-      <c r="G15" s="22" t="s">
+      <c r="G15" s="19" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B16" s="32"/>
-      <c r="C16" s="27" t="s">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B16" s="29"/>
+      <c r="C16" s="24" t="s">
         <v>39</v>
       </c>
-      <c r="D16" s="25">
-        <v>1000</v>
+      <c r="D16" s="22">
+        <f>5*21+4*24+10*31+7*27</f>
+        <v>700</v>
       </c>
       <c r="F16" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B17" s="32"/>
-      <c r="C17" s="27" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="17" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B17" s="29"/>
+      <c r="C17" s="24" t="s">
         <v>40</v>
       </c>
-      <c r="D17" s="25">
+      <c r="D17" s="22">
         <v>200</v>
       </c>
       <c r="F17" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B18" s="31" t="s">
+    <row r="18" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B18" s="28" t="s">
         <v>70</v>
       </c>
-      <c r="C18" s="28"/>
-      <c r="D18" s="29"/>
-      <c r="E18" s="30"/>
-      <c r="F18" s="30"/>
-      <c r="G18" s="30"/>
-    </row>
-    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B19" s="32"/>
-      <c r="C19" s="27" t="s">
+      <c r="C18" s="25"/>
+      <c r="D18" s="26"/>
+      <c r="E18" s="27"/>
+      <c r="F18" s="27"/>
+      <c r="G18" s="27"/>
+    </row>
+    <row r="19" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B19" s="29"/>
+      <c r="C19" s="24" t="s">
         <v>48</v>
       </c>
-      <c r="D19" s="25">
+      <c r="D19" s="22">
         <f>4*37+2*40+2*65</f>
         <v>358</v>
       </c>
       <c r="F19" t="s">
         <v>50</v>
       </c>
-      <c r="G19" s="22" t="s">
+      <c r="G19" s="19" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="20" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B20" s="32"/>
-      <c r="C20" s="27" t="s">
+    <row r="20" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B20" s="29"/>
+      <c r="C20" s="24" t="s">
         <v>49</v>
       </c>
-      <c r="D20" s="25">
+      <c r="D20" s="22">
         <f>2*40+2*65+1*70+1*122</f>
         <v>402</v>
       </c>
@@ -1991,313 +2002,313 @@
         <v>51</v>
       </c>
     </row>
-    <row r="21" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B21" s="32"/>
-      <c r="C21" s="27" t="s">
+    <row r="21" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B21" s="29"/>
+      <c r="C21" s="24" t="s">
         <v>52</v>
       </c>
-      <c r="D21" s="25">
+      <c r="D21" s="22">
         <v>13400</v>
       </c>
       <c r="F21" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="22" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B22" s="33" t="s">
+    <row r="22" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B22" s="30" t="s">
         <v>74</v>
       </c>
-      <c r="C22" s="28"/>
-      <c r="D22" s="29"/>
-      <c r="E22" s="30"/>
-      <c r="F22" s="30"/>
-      <c r="G22" s="30"/>
-    </row>
-    <row r="23" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B23" s="32"/>
-      <c r="C23" s="27" t="s">
+      <c r="C22" s="25"/>
+      <c r="D22" s="26"/>
+      <c r="E22" s="27"/>
+      <c r="F22" s="27"/>
+      <c r="G22" s="27"/>
+    </row>
+    <row r="23" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B23" s="29"/>
+      <c r="C23" s="24" t="s">
         <v>75</v>
       </c>
-      <c r="D23" s="25">
+      <c r="D23" s="22">
         <v>100</v>
       </c>
       <c r="F23" t="s">
         <v>76</v>
       </c>
-      <c r="G23" s="22" t="s">
+      <c r="G23" s="19" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="24" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B24" s="26" t="s">
+    <row r="24" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B24" s="23" t="s">
         <v>18</v>
       </c>
-      <c r="C24" s="30"/>
-      <c r="D24" s="29"/>
-      <c r="E24" s="30"/>
-      <c r="F24" s="30"/>
-      <c r="G24" s="30"/>
-    </row>
-    <row r="25" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B25" s="32"/>
-      <c r="C25" s="27" t="s">
+      <c r="C24" s="27"/>
+      <c r="D24" s="26"/>
+      <c r="E24" s="27"/>
+      <c r="F24" s="27"/>
+      <c r="G24" s="27"/>
+    </row>
+    <row r="25" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B25" s="29"/>
+      <c r="C25" s="24" t="s">
         <v>82</v>
       </c>
-      <c r="D25" s="25">
+      <c r="D25" s="22">
         <f>4*66</f>
         <v>264</v>
       </c>
       <c r="F25" t="s">
         <v>55</v>
       </c>
-      <c r="G25" s="22" t="s">
+      <c r="G25" s="19" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="26" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B26" s="31" t="s">
+    <row r="26" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B26" s="28" t="s">
         <v>69</v>
       </c>
-      <c r="C26" s="30"/>
-      <c r="D26" s="29"/>
-      <c r="E26" s="30"/>
-      <c r="F26" s="30"/>
-      <c r="G26" s="30"/>
-    </row>
-    <row r="27" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B27" s="32"/>
-      <c r="C27" s="27" t="s">
+      <c r="C26" s="27"/>
+      <c r="D26" s="26"/>
+      <c r="E26" s="27"/>
+      <c r="F26" s="27"/>
+      <c r="G26" s="27"/>
+    </row>
+    <row r="27" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B27" s="29"/>
+      <c r="C27" s="24" t="s">
         <v>56</v>
       </c>
-      <c r="D27" s="25">
+      <c r="D27" s="22">
         <v>5000</v>
       </c>
       <c r="F27" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="28" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B28" s="32"/>
-      <c r="C28" s="27" t="s">
+    <row r="28" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B28" s="29"/>
+      <c r="C28" s="24" t="s">
         <v>78</v>
       </c>
-      <c r="D28" s="25">
+      <c r="D28" s="22">
         <f>42+50</f>
         <v>92</v>
       </c>
       <c r="F28" t="s">
         <v>80</v>
       </c>
-      <c r="G28" s="22" t="s">
+      <c r="G28" s="19" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="29" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B29" s="26" t="s">
+    <row r="29" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B29" s="23" t="s">
         <v>28</v>
       </c>
-      <c r="C29" s="30"/>
-      <c r="D29" s="29"/>
-      <c r="E29" s="30"/>
-      <c r="F29" s="30"/>
-      <c r="G29" s="30"/>
-    </row>
-    <row r="30" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B30" s="32"/>
-      <c r="C30" s="27" t="s">
+      <c r="C29" s="27"/>
+      <c r="D29" s="26"/>
+      <c r="E29" s="27"/>
+      <c r="F29" s="27"/>
+      <c r="G29" s="27"/>
+    </row>
+    <row r="30" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B30" s="29"/>
+      <c r="C30" s="24" t="s">
         <v>59</v>
       </c>
-      <c r="D30" s="25">
+      <c r="D30" s="22">
         <f>SUM(D7:D28)</f>
-        <v>23716.35</v>
-      </c>
-    </row>
-    <row r="31" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B31" s="32"/>
-      <c r="C31" s="27" t="s">
+        <v>23416.35</v>
+      </c>
+    </row>
+    <row r="31" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B31" s="29"/>
+      <c r="C31" s="24" t="s">
         <v>58</v>
       </c>
-      <c r="D31" s="25">
+      <c r="D31" s="22">
         <f>D30-D21</f>
-        <v>10316.349999999999</v>
-      </c>
-    </row>
-    <row r="36" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B36" s="1" t="s">
+        <v>10016.349999999999</v>
+      </c>
+    </row>
+    <row r="36" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B36" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="C36" s="2"/>
-      <c r="D36" s="2"/>
-      <c r="E36" s="3"/>
-      <c r="F36" s="4"/>
-      <c r="G36" s="21"/>
-      <c r="H36" s="4"/>
-    </row>
-    <row r="37" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B37" s="5" t="s">
+      <c r="C36" s="32"/>
+      <c r="D36" s="32"/>
+      <c r="E36" s="33"/>
+      <c r="F36" s="2"/>
+      <c r="G36" s="1"/>
+      <c r="H36" s="2"/>
+    </row>
+    <row r="37" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B37" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C37" s="6" t="s">
+      <c r="C37" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D37" s="7" t="s">
+      <c r="D37" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="E37" s="7" t="s">
+      <c r="E37" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="F37" s="8" t="s">
+      <c r="F37" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="G37" s="7"/>
-      <c r="H37" s="8"/>
-    </row>
-    <row r="38" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B38" s="9" t="s">
+      <c r="G37" s="5"/>
+      <c r="H37" s="6"/>
+    </row>
+    <row r="38" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B38" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C38" s="10">
+      <c r="C38" s="8">
         <v>3700</v>
       </c>
-      <c r="D38" s="11" t="s">
+      <c r="D38" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="E38" s="12" t="s">
+      <c r="E38" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="F38" s="13" t="s">
+      <c r="F38" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="G38" s="12"/>
-      <c r="H38" s="13"/>
-    </row>
-    <row r="39" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B39" s="9" t="s">
+      <c r="G38" s="10"/>
+      <c r="H38" s="11"/>
+    </row>
+    <row r="39" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B39" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="C39" s="10">
+      <c r="C39" s="8">
         <v>4200</v>
       </c>
-      <c r="D39" s="11" t="s">
+      <c r="D39" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="E39" s="12" t="s">
+      <c r="E39" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="F39" s="13" t="s">
+      <c r="F39" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="G39" s="12"/>
-      <c r="H39" s="13"/>
-    </row>
-    <row r="40" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B40" s="9" t="s">
+      <c r="G39" s="10"/>
+      <c r="H39" s="11"/>
+    </row>
+    <row r="40" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B40" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="C40" s="10">
+      <c r="C40" s="8">
         <v>400</v>
       </c>
-      <c r="D40" s="11" t="s">
+      <c r="D40" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="E40" s="12" t="s">
+      <c r="E40" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="F40" s="13" t="s">
+      <c r="F40" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="G40" s="12"/>
-      <c r="H40" s="13"/>
-    </row>
-    <row r="41" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B41" s="9" t="s">
+      <c r="G40" s="10"/>
+      <c r="H40" s="11"/>
+    </row>
+    <row r="41" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B41" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="C41" s="10">
+      <c r="C41" s="8">
         <v>300</v>
       </c>
-      <c r="D41" s="11" t="s">
+      <c r="D41" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="E41" s="12" t="s">
+      <c r="E41" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="F41" s="13" t="s">
+      <c r="F41" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="G41" s="12"/>
-      <c r="H41" s="13"/>
-    </row>
-    <row r="42" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B42" s="9" t="s">
+      <c r="G41" s="10"/>
+      <c r="H41" s="11"/>
+    </row>
+    <row r="42" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B42" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="C42" s="10">
+      <c r="C42" s="8">
         <v>900</v>
       </c>
-      <c r="D42" s="11" t="s">
+      <c r="D42" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="E42" s="12" t="s">
+      <c r="E42" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="F42" s="13" t="s">
+      <c r="F42" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="G42" s="12"/>
-      <c r="H42" s="13"/>
-    </row>
-    <row r="43" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B43" s="9" t="s">
+      <c r="G42" s="10"/>
+      <c r="H42" s="11"/>
+    </row>
+    <row r="43" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B43" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="C43" s="10">
+      <c r="C43" s="8">
         <v>5000</v>
       </c>
-      <c r="D43" s="11" t="s">
+      <c r="D43" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="E43" s="12" t="s">
+      <c r="E43" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="F43" s="13" t="s">
+      <c r="F43" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="G43" s="12"/>
-      <c r="H43" s="13"/>
-    </row>
-    <row r="44" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B44" s="14" t="s">
+      <c r="G43" s="10"/>
+      <c r="H43" s="11"/>
+    </row>
+    <row r="44" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B44" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="C44" s="10">
+      <c r="C44" s="8">
         <v>300</v>
       </c>
-      <c r="D44" s="11" t="s">
+      <c r="D44" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="E44" s="12" t="s">
+      <c r="E44" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="F44" s="13" t="s">
+      <c r="F44" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="G44" s="12"/>
-      <c r="H44" s="13"/>
-    </row>
-    <row r="45" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B45" s="15" t="s">
+      <c r="G44" s="10"/>
+      <c r="H44" s="11"/>
+    </row>
+    <row r="45" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B45" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="C45" s="16">
+      <c r="C45" s="14">
         <f>SUBTOTAL(109,Table1[Cost])</f>
         <v>14800</v>
       </c>
-      <c r="D45" s="17"/>
-      <c r="E45" s="18"/>
-      <c r="F45" s="19"/>
-      <c r="G45" s="18"/>
-      <c r="H45" s="19"/>
+      <c r="D45" s="15"/>
+      <c r="E45" s="16"/>
+      <c r="F45" s="17"/>
+      <c r="G45" s="16"/>
+      <c r="H45" s="17"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -2322,25 +2333,25 @@
   <dimension ref="A1:G21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="27.140625" customWidth="1"/>
-    <col min="2" max="2" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="23.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="68.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="27.109375" customWidth="1"/>
+    <col min="2" max="2" width="14.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="68.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="23" t="s">
+    <row r="1" spans="1:7" ht="39.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="20" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C2" t="s">
         <v>72</v>
       </c>
@@ -2357,29 +2368,29 @@
         <v>73</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>53</v>
       </c>
-      <c r="B3" s="26" t="s">
+      <c r="B3" s="23" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="30"/>
-      <c r="D3" s="30"/>
-      <c r="E3" s="30"/>
-      <c r="F3" s="30"/>
-      <c r="G3" s="30"/>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B4" s="32"/>
-      <c r="C4" s="27" t="s">
+      <c r="C3" s="27"/>
+      <c r="D3" s="27"/>
+      <c r="E3" s="27"/>
+      <c r="F3" s="27"/>
+      <c r="G3" s="27"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B4" s="29"/>
+      <c r="C4" s="24" t="s">
         <v>32</v>
       </c>
-      <c r="D4" s="25">
+      <c r="D4" s="22">
         <f>2*120</f>
         <v>240</v>
       </c>
-      <c r="E4" s="25">
+      <c r="E4" s="22">
         <f>D4+D4*0.5</f>
         <v>360</v>
       </c>
@@ -2387,65 +2398,65 @@
         <v>66</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5">
         <f>21+2+2+2+2+1+1+2+2+2+1+1+1+1+1+1+1+6+1+1+1+1+1+5+3</f>
         <v>63</v>
       </c>
-      <c r="B5" s="32"/>
-      <c r="C5" s="27" t="s">
+      <c r="B5" s="29"/>
+      <c r="C5" s="24" t="s">
         <v>30</v>
       </c>
-      <c r="D5" s="24">
+      <c r="D5" s="21">
         <f>80</f>
         <v>80</v>
       </c>
-      <c r="F5" s="20" t="s">
+      <c r="F5" s="18" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B6" s="32"/>
-      <c r="C6" s="27" t="s">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B6" s="29"/>
+      <c r="C6" s="24" t="s">
         <v>60</v>
       </c>
-      <c r="D6" s="24">
+      <c r="D6" s="21">
         <f>55+65+22+97+2*30</f>
         <v>299</v>
       </c>
-      <c r="F6" s="20" t="s">
+      <c r="F6" s="18" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B7" s="26" t="s">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B7" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="C7" s="28"/>
-      <c r="D7" s="29"/>
-      <c r="E7" s="30"/>
-      <c r="F7" s="30"/>
-      <c r="G7" s="30"/>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B8" s="32"/>
-      <c r="C8" s="27" t="s">
+      <c r="C7" s="25"/>
+      <c r="D7" s="26"/>
+      <c r="E7" s="27"/>
+      <c r="F7" s="27"/>
+      <c r="G7" s="27"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B8" s="29"/>
+      <c r="C8" s="24" t="s">
         <v>36</v>
       </c>
-      <c r="D8" s="25">
-        <f>44.95*3*4</f>
-        <v>539.40000000000009</v>
+      <c r="D8" s="22">
+        <f>44.95*2*4</f>
+        <v>359.6</v>
       </c>
       <c r="F8" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B9" s="32"/>
-      <c r="C9" s="27" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B9" s="29"/>
+      <c r="C9" s="24" t="s">
         <v>37</v>
       </c>
-      <c r="D9" s="25">
+      <c r="D9" s="22">
         <f>2.65*63</f>
         <v>166.95</v>
       </c>
@@ -2453,143 +2464,143 @@
         <v>43</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B10" s="32"/>
-      <c r="C10" s="27" t="s">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B10" s="29"/>
+      <c r="C10" s="24" t="s">
         <v>38</v>
       </c>
-      <c r="D10" s="25">
+      <c r="D10" s="22">
         <f>40*12</f>
         <v>480</v>
       </c>
       <c r="F10" t="s">
         <v>42</v>
       </c>
-      <c r="G10" s="22" t="s">
+      <c r="G10" s="19" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B11" s="32"/>
-      <c r="C11" s="27" t="s">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B11" s="29"/>
+      <c r="C11" s="24" t="s">
         <v>39</v>
       </c>
-      <c r="D11" s="25">
+      <c r="D11" s="22">
         <v>1000</v>
       </c>
       <c r="F11" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B12" s="32"/>
-      <c r="C12" s="27" t="s">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B12" s="29"/>
+      <c r="C12" s="24" t="s">
         <v>40</v>
       </c>
-      <c r="D12" s="25">
+      <c r="D12" s="22">
         <v>200</v>
       </c>
       <c r="F12" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B13" s="31" t="s">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B13" s="28" t="s">
         <v>70</v>
       </c>
-      <c r="C13" s="28"/>
-      <c r="D13" s="29"/>
-      <c r="E13" s="30"/>
-      <c r="F13" s="30"/>
-      <c r="G13" s="30"/>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B14" s="32"/>
-      <c r="C14" s="27" t="s">
+      <c r="C13" s="25"/>
+      <c r="D13" s="26"/>
+      <c r="E13" s="27"/>
+      <c r="F13" s="27"/>
+      <c r="G13" s="27"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B14" s="29"/>
+      <c r="C14" s="24" t="s">
         <v>52</v>
       </c>
-      <c r="D14" s="25">
+      <c r="D14" s="22">
         <v>13400</v>
       </c>
       <c r="F14" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B15" s="33" t="s">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B15" s="30" t="s">
         <v>74</v>
       </c>
-      <c r="C15" s="28"/>
-      <c r="D15" s="29"/>
-      <c r="E15" s="30"/>
-      <c r="F15" s="30"/>
-      <c r="G15" s="30"/>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B16" s="32"/>
-      <c r="C16" s="27" t="s">
+      <c r="C15" s="25"/>
+      <c r="D15" s="26"/>
+      <c r="E15" s="27"/>
+      <c r="F15" s="27"/>
+      <c r="G15" s="27"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B16" s="29"/>
+      <c r="C16" s="24" t="s">
         <v>75</v>
       </c>
-      <c r="D16" s="25">
+      <c r="D16" s="22">
         <v>100</v>
       </c>
       <c r="F16" t="s">
         <v>76</v>
       </c>
-      <c r="G16" s="22" t="s">
+      <c r="G16" s="19" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B17" s="31" t="s">
+    <row r="17" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B17" s="28" t="s">
         <v>69</v>
       </c>
-      <c r="C17" s="30"/>
-      <c r="D17" s="29"/>
-      <c r="E17" s="30"/>
-      <c r="F17" s="30"/>
-      <c r="G17" s="30"/>
-    </row>
-    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B18" s="32"/>
-      <c r="C18" s="27" t="s">
+      <c r="C17" s="27"/>
+      <c r="D17" s="26"/>
+      <c r="E17" s="27"/>
+      <c r="F17" s="27"/>
+      <c r="G17" s="27"/>
+    </row>
+    <row r="18" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B18" s="29"/>
+      <c r="C18" s="24" t="s">
         <v>56</v>
       </c>
-      <c r="D18" s="25">
+      <c r="D18" s="22">
         <v>5000</v>
       </c>
       <c r="F18" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B19" s="26" t="s">
+    <row r="19" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B19" s="23" t="s">
         <v>28</v>
       </c>
-      <c r="C19" s="30"/>
-      <c r="D19" s="29"/>
-      <c r="E19" s="30"/>
-      <c r="F19" s="30"/>
-      <c r="G19" s="30"/>
-    </row>
-    <row r="20" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B20" s="32"/>
-      <c r="C20" s="27" t="s">
+      <c r="C19" s="27"/>
+      <c r="D19" s="26"/>
+      <c r="E19" s="27"/>
+      <c r="F19" s="27"/>
+      <c r="G19" s="27"/>
+    </row>
+    <row r="20" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B20" s="29"/>
+      <c r="C20" s="24" t="s">
         <v>59</v>
       </c>
-      <c r="D20" s="25">
+      <c r="D20" s="22">
         <f>SUM(D5:D18)</f>
-        <v>21265.35</v>
-      </c>
-    </row>
-    <row r="21" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B21" s="32"/>
-      <c r="C21" s="27" t="s">
+        <v>21085.55</v>
+      </c>
+    </row>
+    <row r="21" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B21" s="29"/>
+      <c r="C21" s="24" t="s">
         <v>58</v>
       </c>
-      <c r="D21" s="25">
+      <c r="D21" s="22">
         <f>D20-D14</f>
-        <v>7865.3499999999985</v>
+        <v>7685.5499999999993</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
at connectors, moving notes to onenote, budget
</commit_message>
<xml_diff>
--- a/MCHA Budget.xlsx
+++ b/MCHA Budget.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Uni\NU Teams\2025 Lead MCHA\NU-Racing-Lead-MCHA-2025\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5FCB2DA-DB89-40B6-BB0C-E6EE936DE421}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E87DD7E2-7CF4-4D65-99DB-7576DF155923}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{C94B0C8E-4BB7-41BB-BABD-F0454CF43B33}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{C94B0C8E-4BB7-41BB-BABD-F0454CF43B33}"/>
   </bookViews>
   <sheets>
     <sheet name="Splurge Budget" sheetId="3" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="97">
   <si>
     <t>MCHA</t>
   </si>
@@ -184,12 +184,6 @@
     <t>https://www.digikey.com.au/en/products/detail/amphenol-industrial-operations/SLPIRBBPSO1EH/93856862</t>
   </si>
   <si>
-    <t>HVIL surlok &amp;  2 pos conn</t>
-  </si>
-  <si>
-    <t>2x 2 pos big boi conns</t>
-  </si>
-  <si>
     <t>*surlok 8mm connector, 5.7mm ePower-Lite</t>
   </si>
   <si>
@@ -307,9 +301,6 @@
     <t>SPLURGE BUDGET</t>
   </si>
   <si>
-    <t>*mobo, BSPD resistors, BSPD breakout, HFR breakout (experiment with op amps)</t>
-  </si>
-  <si>
     <t>Spare 228</t>
   </si>
   <si>
@@ -326,6 +317,18 @@
   </si>
   <si>
     <t>*2 teensys/board, 4 boards</t>
+  </si>
+  <si>
+    <t>DT connectors on NU24:</t>
+  </si>
+  <si>
+    <t>*mobo (experiment with temp sensing circuit), BSPD resistors, BSPD breakout, HFR breakout (experiment with op amps)</t>
+  </si>
+  <si>
+    <t>HVIL surlok &amp;  2 pos conn OPT A</t>
+  </si>
+  <si>
+    <t>2x 2 pos big boi conns OPT B</t>
   </si>
 </sst>
 </file>
@@ -1278,44 +1281,44 @@
   <dimension ref="A1:G33"/>
   <sheetViews>
     <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="F32" sqref="F32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="26.5546875" customWidth="1"/>
     <col min="2" max="2" width="14.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="23.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.77734375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.44140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="73.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="37.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="20" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C2" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D2" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="E2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="F2" t="s">
         <v>3</v>
       </c>
       <c r="G2" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B3" s="23" t="s">
         <v>6</v>
@@ -1333,14 +1336,18 @@
       </c>
       <c r="B4" s="29"/>
       <c r="C4" s="24" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D4" s="22">
         <f>60</f>
         <v>60</v>
       </c>
+      <c r="E4" s="22">
+        <f>D4</f>
+        <v>60</v>
+      </c>
       <c r="F4" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
@@ -1352,8 +1359,12 @@
         <f>60+30</f>
         <v>90</v>
       </c>
+      <c r="E5" s="22">
+        <f>D5*1.5</f>
+        <v>135</v>
+      </c>
       <c r="F5" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
@@ -1366,11 +1377,11 @@
         <v>240</v>
       </c>
       <c r="E6" s="22">
-        <f>D6+D6*0.5</f>
+        <f>D6*1.5</f>
         <v>360</v>
       </c>
       <c r="F6" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
@@ -1382,21 +1393,29 @@
         <f>80+35+60+90*2</f>
         <v>355</v>
       </c>
+      <c r="E7" s="22">
+        <f>D7*2</f>
+        <v>710</v>
+      </c>
       <c r="F7" s="18" t="s">
-        <v>89</v>
+        <v>94</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B8" s="29"/>
       <c r="C8" s="24" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D8" s="21">
         <f>55+65+22+97+2*30</f>
         <v>299</v>
       </c>
+      <c r="E8" s="22">
+        <f>D8*1.5</f>
+        <v>448.5</v>
+      </c>
       <c r="F8" s="18" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
@@ -1408,8 +1427,12 @@
         <f>3*80+30</f>
         <v>270</v>
       </c>
+      <c r="E9" s="22">
+        <f>D9*2</f>
+        <v>540</v>
+      </c>
       <c r="F9" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
@@ -1420,6 +1443,10 @@
       <c r="D10" s="22">
         <v>800</v>
       </c>
+      <c r="E10" s="22">
+        <f>D10</f>
+        <v>800</v>
+      </c>
       <c r="F10" t="s">
         <v>46</v>
       </c>
@@ -1432,8 +1459,12 @@
       <c r="D11" s="22">
         <v>200</v>
       </c>
+      <c r="E11" s="22">
+        <f>D11</f>
+        <v>200</v>
+      </c>
       <c r="F11" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
@@ -1455,6 +1486,10 @@
         <f>44.95*3*4</f>
         <v>539.40000000000009</v>
       </c>
+      <c r="E13" s="22">
+        <f>D13*1.25</f>
+        <v>674.25000000000011</v>
+      </c>
       <c r="F13" t="s">
         <v>44</v>
       </c>
@@ -1468,6 +1503,10 @@
         <f>2.65*63</f>
         <v>166.95</v>
       </c>
+      <c r="E14" s="22">
+        <f>D14*1</f>
+        <v>166.95</v>
+      </c>
       <c r="F14" t="s">
         <v>43</v>
       </c>
@@ -1481,6 +1520,10 @@
         <f>40*12</f>
         <v>480</v>
       </c>
+      <c r="E15" s="22">
+        <f>D15*1.5</f>
+        <v>720</v>
+      </c>
       <c r="F15" t="s">
         <v>42</v>
       </c>
@@ -1497,8 +1540,12 @@
         <f>5*21+4*24+10*31+7*27+300</f>
         <v>1000</v>
       </c>
+      <c r="E16" s="22">
+        <f>D16*1.5</f>
+        <v>1500</v>
+      </c>
       <c r="F16" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
     </row>
     <row r="17" spans="2:7" x14ac:dyDescent="0.3">
@@ -1509,13 +1556,17 @@
       <c r="D17" s="22">
         <v>200</v>
       </c>
+      <c r="E17" s="22">
+        <f>D17</f>
+        <v>200</v>
+      </c>
       <c r="F17" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="18" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B18" s="28" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C18" s="25"/>
       <c r="D18" s="26"/>
@@ -1526,14 +1577,18 @@
     <row r="19" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B19" s="29"/>
       <c r="C19" s="24" t="s">
-        <v>48</v>
+        <v>95</v>
       </c>
       <c r="D19" s="22">
         <f>4*37+2*40+2*65</f>
         <v>358</v>
       </c>
+      <c r="E19" s="22">
+        <f>D19*1.5</f>
+        <v>537</v>
+      </c>
       <c r="F19" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="G19" s="19" t="s">
         <v>47</v>
@@ -1542,43 +1597,55 @@
     <row r="20" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B20" s="29"/>
       <c r="C20" s="24" t="s">
-        <v>49</v>
+        <v>96</v>
       </c>
       <c r="D20" s="22">
         <f>2*40+2*65+1*70+1*122</f>
         <v>402</v>
       </c>
+      <c r="E20" s="22">
+        <f>D20*2</f>
+        <v>804</v>
+      </c>
       <c r="F20" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="21" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B21" s="29"/>
       <c r="C21" s="24" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D21" s="22">
         <v>13400</v>
       </c>
+      <c r="E21" s="22">
+        <f>D21</f>
+        <v>13400</v>
+      </c>
       <c r="F21" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="22" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B22" s="29"/>
       <c r="C22" s="24" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="D22" s="22">
         <v>6500</v>
       </c>
+      <c r="E22" s="22">
+        <f>D22</f>
+        <v>6500</v>
+      </c>
       <c r="F22" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
     </row>
     <row r="23" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B23" s="30" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C23" s="25"/>
       <c r="D23" s="26"/>
@@ -1589,16 +1656,20 @@
     <row r="24" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B24" s="29"/>
       <c r="C24" s="24" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="D24" s="22">
         <v>100</v>
       </c>
+      <c r="E24" s="22">
+        <f>D24*2</f>
+        <v>200</v>
+      </c>
       <c r="F24" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="G24" s="19" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="25" spans="2:7" x14ac:dyDescent="0.3">
@@ -1614,22 +1685,26 @@
     <row r="26" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B26" s="29"/>
       <c r="C26" s="24" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D26" s="22">
         <f>4*66</f>
         <v>264</v>
       </c>
+      <c r="E26" s="22">
+        <f>D26*1.25</f>
+        <v>330</v>
+      </c>
       <c r="F26" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="G26" s="19" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="27" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B27" s="28" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C27" s="27"/>
       <c r="D27" s="26"/>
@@ -1640,29 +1715,37 @@
     <row r="28" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B28" s="29"/>
       <c r="C28" s="24" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D28" s="22">
         <v>5000</v>
       </c>
+      <c r="E28" s="22">
+        <f>D28</f>
+        <v>5000</v>
+      </c>
       <c r="F28" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="29" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B29" s="29"/>
       <c r="C29" s="24" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="D29" s="22">
         <f>42+50</f>
         <v>92</v>
       </c>
+      <c r="E29" s="22">
+        <f>D29*1.25</f>
+        <v>115</v>
+      </c>
       <c r="F29" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="G29" s="19" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="30" spans="2:7" x14ac:dyDescent="0.3">
@@ -1678,31 +1761,43 @@
     <row r="31" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B31" s="29"/>
       <c r="C31" s="24" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D31" s="22">
         <f>SUM(D4:D29)</f>
         <v>30816.35</v>
       </c>
+      <c r="E31" s="22">
+        <f>SUM(E4:E29)</f>
+        <v>33400.699999999997</v>
+      </c>
     </row>
     <row r="32" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B32" s="29"/>
       <c r="C32" s="24" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D32" s="22">
         <f>D31-D21</f>
         <v>17416.349999999999</v>
       </c>
-    </row>
-    <row r="33" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="E32" s="22">
+        <f>E31-E21</f>
+        <v>20000.699999999997</v>
+      </c>
+    </row>
+    <row r="33" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B33" s="29"/>
       <c r="C33" s="24" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="D33" s="22">
         <f>D31-D22-D21</f>
         <v>10916.349999999999</v>
+      </c>
+      <c r="E33" s="22">
+        <f>E31-E22-E21</f>
+        <v>13500.699999999997</v>
       </c>
     </row>
   </sheetData>
@@ -1721,15 +1816,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C2DAFC3-A69B-479A-8EED-66262DCE6CA9}">
   <dimension ref="A1:H45"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="26.6640625" customWidth="1"/>
     <col min="2" max="2" width="17.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="23.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.77734375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="16.6640625" customWidth="1"/>
     <col min="5" max="5" width="10.44140625" customWidth="1"/>
     <col min="6" max="6" width="68.6640625" bestFit="1" customWidth="1"/>
@@ -1744,29 +1839,29 @@
   <sheetData>
     <row r="1" spans="1:7" ht="36.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="20" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C2" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D2" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="E2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="F2" t="s">
         <v>3</v>
       </c>
       <c r="G2" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B3" s="23" t="s">
         <v>6</v>
@@ -1780,13 +1875,13 @@
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B4" s="29"/>
       <c r="C4" s="24" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D4" s="22">
         <v>60</v>
       </c>
       <c r="F4" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
@@ -1799,7 +1894,7 @@
         <v>90</v>
       </c>
       <c r="F5" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
@@ -1816,7 +1911,7 @@
         <v>360</v>
       </c>
       <c r="F6" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
@@ -1833,20 +1928,20 @@
         <v>175</v>
       </c>
       <c r="F7" s="18" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B8" s="29"/>
       <c r="C8" s="24" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D8" s="21">
         <f>55+65+22+97+2*30</f>
         <v>299</v>
       </c>
       <c r="F8" s="18" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
@@ -1859,7 +1954,7 @@
         <v>240</v>
       </c>
       <c r="F9" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
@@ -1883,7 +1978,7 @@
         <v>200</v>
       </c>
       <c r="F11" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
@@ -1948,7 +2043,7 @@
         <v>700</v>
       </c>
       <c r="F16" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
     </row>
     <row r="17" spans="2:7" x14ac:dyDescent="0.3">
@@ -1965,7 +2060,7 @@
     </row>
     <row r="18" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B18" s="28" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C18" s="25"/>
       <c r="D18" s="26"/>
@@ -1976,14 +2071,14 @@
     <row r="19" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B19" s="29"/>
       <c r="C19" s="24" t="s">
-        <v>48</v>
+        <v>95</v>
       </c>
       <c r="D19" s="22">
         <f>4*37+2*40+2*65</f>
         <v>358</v>
       </c>
       <c r="F19" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="G19" s="19" t="s">
         <v>47</v>
@@ -1992,31 +2087,31 @@
     <row r="20" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B20" s="29"/>
       <c r="C20" s="24" t="s">
-        <v>49</v>
+        <v>96</v>
       </c>
       <c r="D20" s="22">
         <f>2*40+2*65+1*70+1*122</f>
         <v>402</v>
       </c>
       <c r="F20" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="21" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B21" s="29"/>
       <c r="C21" s="24" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D21" s="22">
         <v>13400</v>
       </c>
       <c r="F21" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="22" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B22" s="30" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C22" s="25"/>
       <c r="D22" s="26"/>
@@ -2027,16 +2122,16 @@
     <row r="23" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B23" s="29"/>
       <c r="C23" s="24" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="D23" s="22">
         <v>100</v>
       </c>
       <c r="F23" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="G23" s="19" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="24" spans="2:7" x14ac:dyDescent="0.3">
@@ -2052,22 +2147,22 @@
     <row r="25" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B25" s="29"/>
       <c r="C25" s="24" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D25" s="22">
         <f>4*66</f>
         <v>264</v>
       </c>
       <c r="F25" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="G25" s="19" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="26" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B26" s="28" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C26" s="27"/>
       <c r="D26" s="26"/>
@@ -2078,29 +2173,29 @@
     <row r="27" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B27" s="29"/>
       <c r="C27" s="24" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D27" s="22">
         <v>5000</v>
       </c>
       <c r="F27" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="28" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B28" s="29"/>
       <c r="C28" s="24" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="D28" s="22">
         <f>42+50</f>
         <v>92</v>
       </c>
       <c r="F28" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="G28" s="19" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="29" spans="2:7" x14ac:dyDescent="0.3">
@@ -2116,7 +2211,7 @@
     <row r="30" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B30" s="29"/>
       <c r="C30" s="24" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D30" s="22">
         <f>SUM(D7:D28)</f>
@@ -2126,7 +2221,7 @@
     <row r="31" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B31" s="29"/>
       <c r="C31" s="24" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D31" s="22">
         <f>D30-D21</f>
@@ -2332,8 +2427,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73C411A0-DC73-430D-BB94-0FCD773FE51F}">
   <dimension ref="A1:G21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2348,29 +2443,29 @@
   <sheetData>
     <row r="1" spans="1:7" ht="39.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="20" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C2" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D2" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="E2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="F2" t="s">
         <v>3</v>
       </c>
       <c r="G2" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>53</v>
+        <v>93</v>
       </c>
       <c r="B3" s="23" t="s">
         <v>6</v>
@@ -2382,6 +2477,10 @@
       <c r="G3" s="27"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <f>21+2+2+2+2+1+1+2+2+2+1+1+1+1+1+1+1+6+1+1+1+1+1+5+3</f>
+        <v>63</v>
+      </c>
       <c r="B4" s="29"/>
       <c r="C4" s="24" t="s">
         <v>32</v>
@@ -2395,14 +2494,10 @@
         <v>360</v>
       </c>
       <c r="F4" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A5">
-        <f>21+2+2+2+2+1+1+2+2+2+1+1+1+1+1+1+1+6+1+1+1+1+1+5+3</f>
-        <v>63</v>
-      </c>
       <c r="B5" s="29"/>
       <c r="C5" s="24" t="s">
         <v>30</v>
@@ -2412,20 +2507,20 @@
         <v>80</v>
       </c>
       <c r="F5" s="18" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B6" s="29"/>
       <c r="C6" s="24" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D6" s="21">
         <f>55+65+22+97+2*30</f>
         <v>299</v>
       </c>
       <c r="F6" s="18" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
@@ -2448,7 +2543,7 @@
         <v>359.6</v>
       </c>
       <c r="F8" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
@@ -2506,7 +2601,7 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B13" s="28" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C13" s="25"/>
       <c r="D13" s="26"/>
@@ -2517,18 +2612,18 @@
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B14" s="29"/>
       <c r="C14" s="24" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D14" s="22">
         <v>13400</v>
       </c>
       <c r="F14" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B15" s="30" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C15" s="25"/>
       <c r="D15" s="26"/>
@@ -2539,21 +2634,21 @@
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B16" s="29"/>
       <c r="C16" s="24" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="D16" s="22">
         <v>100</v>
       </c>
       <c r="F16" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="G16" s="19" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="17" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B17" s="28" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C17" s="27"/>
       <c r="D17" s="26"/>
@@ -2564,13 +2659,13 @@
     <row r="18" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B18" s="29"/>
       <c r="C18" s="24" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D18" s="22">
         <v>5000</v>
       </c>
       <c r="F18" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="19" spans="2:7" x14ac:dyDescent="0.3">
@@ -2586,7 +2681,7 @@
     <row r="20" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B20" s="29"/>
       <c r="C20" s="24" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D20" s="22">
         <f>SUM(D5:D18)</f>
@@ -2596,7 +2691,7 @@
     <row r="21" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B21" s="29"/>
       <c r="C21" s="24" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D21" s="22">
         <f>D20-D14</f>

</xml_diff>